<commit_message>
Sample template Cypress and BC Law process changed
Sample template Cypress and BC Law process changed
</commit_message>
<xml_diff>
--- a/public/template/BC Law Firm_sample_template.xlsx
+++ b/public/template/BC Law Firm_sample_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stellar-oms(dev)\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AE3523-0B15-4DAD-A6C5-CC5BC03C103F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE529C07-2E13-4CBD-A7BD-E110A860ECA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -98,9 +98,6 @@
     <t>Process</t>
   </si>
   <si>
-    <t>Search</t>
-  </si>
-  <si>
     <t>Client</t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Update Search</t>
+  </si>
+  <si>
+    <t>Search &amp; Typing</t>
   </si>
 </sst>
 </file>
@@ -990,7 +990,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1019,7 +1019,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>15</v>
@@ -1060,16 +1060,16 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>8</v>
@@ -1101,16 +1101,16 @@
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Bulk sample typist and typist_qc added and also in manual
Bulk sample typist and typist_qc added and also in manual
</commit_message>
<xml_diff>
--- a/public/template/BC Law Firm_sample_template.xlsx
+++ b/public/template/BC Law Firm_sample_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stellar-oms(dev)\public\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE529C07-2E13-4CBD-A7BD-E110A860ECA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51916ABF-33BE-4DB1-B13B-5743F66DA238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>Order Received Data and Time</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Status</t>
   </si>
   <si>
-    <t>SIPL0004</t>
-  </si>
-  <si>
     <t>FL</t>
   </si>
   <si>
@@ -71,30 +68,12 @@
     <t>WIP</t>
   </si>
   <si>
-    <t>Tier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search(T1) </t>
-  </si>
-  <si>
-    <t>Search(T2)</t>
-  </si>
-  <si>
-    <t>SIPL0005</t>
-  </si>
-  <si>
     <t>Product Name</t>
   </si>
   <si>
     <t>Lob</t>
   </si>
   <si>
-    <t>Municipality</t>
-  </si>
-  <si>
-    <t>FLClay</t>
-  </si>
-  <si>
     <t>Process</t>
   </si>
   <si>
@@ -114,6 +93,36 @@
   </si>
   <si>
     <t>Search &amp; Typing</t>
+  </si>
+  <si>
+    <t>Typist</t>
+  </si>
+  <si>
+    <t>Typist QC</t>
+  </si>
+  <si>
+    <t>SIPL5316</t>
+  </si>
+  <si>
+    <t>SIPL5688</t>
+  </si>
+  <si>
+    <t>SIPL0102</t>
+  </si>
+  <si>
+    <t>SIPL0103</t>
+  </si>
+  <si>
+    <t>Current Owner Search</t>
+  </si>
+  <si>
+    <t>001BC</t>
+  </si>
+  <si>
+    <t>002BC</t>
+  </si>
+  <si>
+    <t>003BC</t>
   </si>
 </sst>
 </file>
@@ -123,7 +132,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -264,6 +273,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -452,7 +468,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -582,6 +598,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -627,11 +656,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -987,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,9 +1031,9 @@
     <col min="3" max="3" width="36.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="8" width="16" customWidth="1"/>
+    <col min="6" max="7" width="16" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
     <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -1019,113 +1050,154 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>15</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45436</v>
       </c>
-      <c r="B2" s="1">
-        <v>13286</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45439</v>
       </c>
-      <c r="B3" s="1">
-        <v>219289</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+      <c r="B3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>45439</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="F4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="K4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>